<commit_message>
Updated trade data, adjusted recession shading
</commit_message>
<xml_diff>
--- a/data/exh1.xlsx
+++ b/data/exh1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\econ019fs\ftd53\TDSB2\Internet\Current\Press-Release\current_press_release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41CBAA1E-A80F-453E-B078-264C099D0AFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BD72110-E489-4E19-9B76-5935F8C50E72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{072694D4-AD59-4E37-8687-4566B6C0AB92}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EC54B424-AE5E-4254-86B3-540590A5AB81}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -132,7 +132,7 @@
     <t>Jan. - Dec.</t>
   </si>
   <si>
-    <t>Jan. - Mar.</t>
+    <t>Jan. - May</t>
   </si>
   <si>
     <t>January</t>
@@ -177,13 +177,13 @@
     <t>2021</t>
   </si>
   <si>
-    <t>February (R)</t>
+    <t>April (R)</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>February data as published last month:</t>
+    <t>April data as published last month:</t>
   </si>
   <si>
     <t>(1) Data are presented on a balance of payments (BOP) basis.</t>
@@ -56778,7 +56778,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFEBAD79-1EE0-4591-8712-C6D63A0987E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADEFEE79-7FAD-4FFB-A248-5DDFC04957F5}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -57099,31 +57099,31 @@
         <v>12</v>
       </c>
       <c r="B8" s="27">
-        <v>-576865</v>
+        <v>-576341</v>
       </c>
       <c r="C8" s="27">
-        <v>-864331</v>
+        <v>-861515</v>
       </c>
       <c r="D8" s="28">
-        <v>287466</v>
+        <v>285174</v>
       </c>
       <c r="E8" s="29">
-        <v>2528262</v>
+        <v>2528367</v>
       </c>
       <c r="F8" s="27">
-        <v>1652437</v>
+        <v>1652072</v>
       </c>
       <c r="G8" s="30">
-        <v>875825</v>
+        <v>876295</v>
       </c>
       <c r="H8" s="31">
-        <v>3105127</v>
+        <v>3104708</v>
       </c>
       <c r="I8" s="27">
-        <v>2516767</v>
+        <v>2513587</v>
       </c>
       <c r="J8" s="28">
-        <v>588359</v>
+        <v>591121</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57131,31 +57131,31 @@
         <v>13</v>
       </c>
       <c r="B9" s="33">
-        <v>-145237</v>
+        <v>-248605</v>
       </c>
       <c r="C9" s="33">
-        <v>-216133</v>
+        <v>-367685</v>
       </c>
       <c r="D9" s="34">
-        <v>70895</v>
+        <v>119080</v>
       </c>
       <c r="E9" s="35">
-        <v>634210</v>
+        <v>1057295</v>
       </c>
       <c r="F9" s="33">
-        <v>419048</v>
+        <v>694430</v>
       </c>
       <c r="G9" s="36">
-        <v>215162</v>
+        <v>362865</v>
       </c>
       <c r="H9" s="37">
-        <v>779447</v>
+        <v>1305900</v>
       </c>
       <c r="I9" s="33">
-        <v>635180</v>
+        <v>1062115</v>
       </c>
       <c r="J9" s="34">
-        <v>144267</v>
+        <v>243785</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -57163,31 +57163,31 @@
         <v>14</v>
       </c>
       <c r="B10" s="27">
-        <v>-49023</v>
+        <v>-48818</v>
       </c>
       <c r="C10" s="27">
-        <v>-72369</v>
+        <v>-72422</v>
       </c>
       <c r="D10" s="28">
-        <v>23346</v>
+        <v>23604</v>
       </c>
       <c r="E10" s="29">
-        <v>210243</v>
+        <v>209087</v>
       </c>
       <c r="F10" s="27">
-        <v>138878</v>
+        <v>137716</v>
       </c>
       <c r="G10" s="30">
-        <v>71366</v>
+        <v>71371</v>
       </c>
       <c r="H10" s="31">
-        <v>259267</v>
+        <v>257905</v>
       </c>
       <c r="I10" s="27">
-        <v>211247</v>
+        <v>210138</v>
       </c>
       <c r="J10" s="28">
-        <v>48020</v>
+        <v>47768</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57195,31 +57195,31 @@
         <v>15</v>
       </c>
       <c r="B11" s="27">
-        <v>-47300</v>
+        <v>-48032</v>
       </c>
       <c r="C11" s="27">
-        <v>-71032</v>
+        <v>-71831</v>
       </c>
       <c r="D11" s="28">
-        <v>23732</v>
+        <v>23799</v>
       </c>
       <c r="E11" s="29">
-        <v>210809</v>
+        <v>210133</v>
       </c>
       <c r="F11" s="27">
-        <v>139190</v>
+        <v>138255</v>
       </c>
       <c r="G11" s="30">
-        <v>71619</v>
+        <v>71878</v>
       </c>
       <c r="H11" s="31">
-        <v>258109</v>
+        <v>258165</v>
       </c>
       <c r="I11" s="27">
-        <v>210222</v>
+        <v>210086</v>
       </c>
       <c r="J11" s="28">
-        <v>47887</v>
+        <v>48079</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57227,31 +57227,31 @@
         <v>16</v>
       </c>
       <c r="B12" s="27">
-        <v>-48914</v>
+        <v>-49777</v>
       </c>
       <c r="C12" s="27">
-        <v>-72732</v>
+        <v>-73355</v>
       </c>
       <c r="D12" s="28">
-        <v>23817</v>
+        <v>23578</v>
       </c>
       <c r="E12" s="29">
-        <v>213157</v>
+        <v>213813</v>
       </c>
       <c r="F12" s="27">
-        <v>140980</v>
+        <v>141183</v>
       </c>
       <c r="G12" s="30">
-        <v>72177</v>
+        <v>72630</v>
       </c>
       <c r="H12" s="31">
-        <v>262072</v>
+        <v>263590</v>
       </c>
       <c r="I12" s="27">
-        <v>213712</v>
+        <v>214538</v>
       </c>
       <c r="J12" s="28">
-        <v>48360</v>
+        <v>49052</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57259,31 +57259,31 @@
         <v>17</v>
       </c>
       <c r="B13" s="27">
-        <v>-49203</v>
+        <v>-50074</v>
       </c>
       <c r="C13" s="27">
-        <v>-73312</v>
+        <v>-73654</v>
       </c>
       <c r="D13" s="28">
-        <v>24109</v>
+        <v>23580</v>
       </c>
       <c r="E13" s="29">
-        <v>209288</v>
+        <v>210289</v>
       </c>
       <c r="F13" s="27">
-        <v>136436</v>
+        <v>137284</v>
       </c>
       <c r="G13" s="30">
-        <v>72852</v>
+        <v>73005</v>
       </c>
       <c r="H13" s="31">
-        <v>258491</v>
+        <v>260363</v>
       </c>
       <c r="I13" s="27">
-        <v>209748</v>
+        <v>210937</v>
       </c>
       <c r="J13" s="28">
-        <v>48743</v>
+        <v>49425</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57291,31 +57291,31 @@
         <v>18</v>
       </c>
       <c r="B14" s="27">
-        <v>-51258</v>
+        <v>-51904</v>
       </c>
       <c r="C14" s="27">
-        <v>-75962</v>
+        <v>-76423</v>
       </c>
       <c r="D14" s="28">
-        <v>24704</v>
+        <v>24520</v>
       </c>
       <c r="E14" s="29">
-        <v>212852</v>
+        <v>213973</v>
       </c>
       <c r="F14" s="27">
-        <v>139091</v>
+        <v>139993</v>
       </c>
       <c r="G14" s="30">
-        <v>73761</v>
+        <v>73980</v>
       </c>
       <c r="H14" s="31">
-        <v>264110</v>
+        <v>265877</v>
       </c>
       <c r="I14" s="27">
-        <v>215053</v>
+        <v>216416</v>
       </c>
       <c r="J14" s="28">
-        <v>49057</v>
+        <v>49461</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57323,31 +57323,31 @@
         <v>19</v>
       </c>
       <c r="B15" s="27">
-        <v>-51749</v>
+        <v>-50390</v>
       </c>
       <c r="C15" s="27">
-        <v>-75298</v>
+        <v>-74285</v>
       </c>
       <c r="D15" s="28">
-        <v>23549</v>
+        <v>23895</v>
       </c>
       <c r="E15" s="29">
-        <v>209254</v>
+        <v>210575</v>
       </c>
       <c r="F15" s="27">
-        <v>135542</v>
+        <v>136744</v>
       </c>
       <c r="G15" s="30">
-        <v>73712</v>
+        <v>73831</v>
       </c>
       <c r="H15" s="31">
-        <v>261003</v>
+        <v>260965</v>
       </c>
       <c r="I15" s="27">
-        <v>210839</v>
+        <v>211029</v>
       </c>
       <c r="J15" s="28">
-        <v>50164</v>
+        <v>49936</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -57355,31 +57355,31 @@
         <v>20</v>
       </c>
       <c r="B16" s="27">
-        <v>-51041</v>
+        <v>-49959</v>
       </c>
       <c r="C16" s="27">
-        <v>-74606</v>
+        <v>-73237</v>
       </c>
       <c r="D16" s="28">
-        <v>23565</v>
+        <v>23277</v>
       </c>
       <c r="E16" s="29">
-        <v>210462</v>
+        <v>211469</v>
       </c>
       <c r="F16" s="27">
-        <v>137465</v>
+        <v>138532</v>
       </c>
       <c r="G16" s="30">
-        <v>72997</v>
+        <v>72937</v>
       </c>
       <c r="H16" s="31">
-        <v>261503</v>
+        <v>261428</v>
       </c>
       <c r="I16" s="27">
-        <v>212071</v>
+        <v>211768</v>
       </c>
       <c r="J16" s="28">
-        <v>49432</v>
+        <v>49660</v>
       </c>
     </row>
     <row r="17" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57387,31 +57387,31 @@
         <v>21</v>
       </c>
       <c r="B17" s="27">
-        <v>-50778</v>
+        <v>-50388</v>
       </c>
       <c r="C17" s="27">
-        <v>-74598</v>
+        <v>-73758</v>
       </c>
       <c r="D17" s="28">
-        <v>23820</v>
+        <v>23369</v>
       </c>
       <c r="E17" s="29">
-        <v>210517</v>
+        <v>210474</v>
       </c>
       <c r="F17" s="27">
-        <v>137358</v>
+        <v>137434</v>
       </c>
       <c r="G17" s="30">
-        <v>73159</v>
+        <v>73040</v>
       </c>
       <c r="H17" s="31">
-        <v>261295</v>
+        <v>260862</v>
       </c>
       <c r="I17" s="27">
-        <v>211956</v>
+        <v>211192</v>
       </c>
       <c r="J17" s="28">
-        <v>49339</v>
+        <v>49671</v>
       </c>
     </row>
     <row r="18" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57419,31 +57419,31 @@
         <v>22</v>
       </c>
       <c r="B18" s="27">
-        <v>-47839</v>
+        <v>-48262</v>
       </c>
       <c r="C18" s="27">
-        <v>-71925</v>
+        <v>-71377</v>
       </c>
       <c r="D18" s="28">
-        <v>24085</v>
+        <v>23115</v>
       </c>
       <c r="E18" s="29">
-        <v>209210</v>
+        <v>208776</v>
       </c>
       <c r="F18" s="27">
-        <v>136108</v>
+        <v>135806</v>
       </c>
       <c r="G18" s="30">
-        <v>73102</v>
+        <v>72970</v>
       </c>
       <c r="H18" s="31">
-        <v>257049</v>
+        <v>257037</v>
       </c>
       <c r="I18" s="27">
-        <v>208032</v>
+        <v>207183</v>
       </c>
       <c r="J18" s="28">
-        <v>49017</v>
+        <v>49854</v>
       </c>
     </row>
     <row r="19" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57451,31 +57451,31 @@
         <v>23</v>
       </c>
       <c r="B19" s="27">
-        <v>-43029</v>
+        <v>-42720</v>
       </c>
       <c r="C19" s="27">
-        <v>-67131</v>
+        <v>-67038</v>
       </c>
       <c r="D19" s="28">
-        <v>24102</v>
+        <v>24318</v>
       </c>
       <c r="E19" s="29">
-        <v>210403</v>
+        <v>210157</v>
       </c>
       <c r="F19" s="27">
-        <v>136851</v>
+        <v>136299</v>
       </c>
       <c r="G19" s="30">
-        <v>73552</v>
+        <v>73857</v>
       </c>
       <c r="H19" s="31">
-        <v>253432</v>
+        <v>252877</v>
       </c>
       <c r="I19" s="27">
-        <v>203982</v>
+        <v>203338</v>
       </c>
       <c r="J19" s="28">
-        <v>49449</v>
+        <v>49539</v>
       </c>
     </row>
     <row r="20" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57483,31 +57483,31 @@
         <v>24</v>
       </c>
       <c r="B20" s="27">
-        <v>-41054</v>
+        <v>-40596</v>
       </c>
       <c r="C20" s="27">
-        <v>-65391</v>
+        <v>-64945</v>
       </c>
       <c r="D20" s="28">
-        <v>24337</v>
+        <v>24349</v>
       </c>
       <c r="E20" s="29">
-        <v>210571</v>
+        <v>209739</v>
       </c>
       <c r="F20" s="27">
-        <v>136888</v>
+        <v>136127</v>
       </c>
       <c r="G20" s="30">
-        <v>73682</v>
+        <v>73611</v>
       </c>
       <c r="H20" s="31">
-        <v>251625</v>
+        <v>250335</v>
       </c>
       <c r="I20" s="27">
-        <v>202280</v>
+        <v>201072</v>
       </c>
       <c r="J20" s="28">
-        <v>49345</v>
+        <v>49263</v>
       </c>
       <c r="K20" s="38"/>
       <c r="L20" s="38"/>
@@ -57738,31 +57738,31 @@
         <v>25</v>
       </c>
       <c r="B21" s="27">
-        <v>-45676</v>
+        <v>-45421</v>
       </c>
       <c r="C21" s="27">
-        <v>-69975</v>
+        <v>-69191</v>
       </c>
       <c r="D21" s="28">
-        <v>24299</v>
+        <v>23769</v>
       </c>
       <c r="E21" s="29">
-        <v>211496</v>
+        <v>209883</v>
       </c>
       <c r="F21" s="27">
-        <v>137651</v>
+        <v>136699</v>
       </c>
       <c r="G21" s="30">
-        <v>73845</v>
+        <v>73184</v>
       </c>
       <c r="H21" s="31">
-        <v>257171</v>
+        <v>255304</v>
       </c>
       <c r="I21" s="27">
-        <v>207625</v>
+        <v>205889</v>
       </c>
       <c r="J21" s="28">
-        <v>49546</v>
+        <v>49415</v>
       </c>
     </row>
     <row r="22" spans="1:233" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -57784,31 +57784,31 @@
         <v>12</v>
       </c>
       <c r="B23" s="27">
-        <v>-681700</v>
+        <v>-676684</v>
       </c>
       <c r="C23" s="27">
-        <v>-915570</v>
+        <v>-922026</v>
       </c>
       <c r="D23" s="28">
-        <v>233870</v>
+        <v>245342</v>
       </c>
       <c r="E23" s="29">
-        <v>2127254</v>
+        <v>2134441</v>
       </c>
       <c r="F23" s="27">
-        <v>1435128</v>
+        <v>1428798</v>
       </c>
       <c r="G23" s="30">
-        <v>692126</v>
+        <v>705643</v>
       </c>
       <c r="H23" s="31">
-        <v>2808954</v>
+        <v>2811125</v>
       </c>
       <c r="I23" s="27">
-        <v>2350698</v>
+        <v>2350825</v>
       </c>
       <c r="J23" s="28">
-        <v>458256</v>
+        <v>460301</v>
       </c>
     </row>
     <row r="24" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57816,31 +57816,31 @@
         <v>13</v>
       </c>
       <c r="B24" s="33">
-        <v>-129630</v>
+        <v>-242122</v>
       </c>
       <c r="C24" s="33">
-        <v>-193681</v>
+        <v>-351527</v>
       </c>
       <c r="D24" s="34">
-        <v>64051</v>
+        <v>109405</v>
       </c>
       <c r="E24" s="35">
-        <v>600844</v>
+        <v>893582</v>
       </c>
       <c r="F24" s="33">
-        <v>402910</v>
+        <v>584220</v>
       </c>
       <c r="G24" s="36">
-        <v>197934</v>
+        <v>309362</v>
       </c>
       <c r="H24" s="37">
-        <v>730474</v>
+        <v>1135704</v>
       </c>
       <c r="I24" s="33">
-        <v>596591</v>
+        <v>935747</v>
       </c>
       <c r="J24" s="34">
-        <v>133883</v>
+        <v>199958</v>
       </c>
     </row>
     <row r="25" spans="1:233" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -57848,31 +57848,31 @@
         <v>14</v>
       </c>
       <c r="B25" s="27">
-        <v>-44379</v>
+        <v>-45452</v>
       </c>
       <c r="C25" s="27">
-        <v>-66772</v>
+        <v>-67839</v>
       </c>
       <c r="D25" s="28">
-        <v>22393</v>
+        <v>22387</v>
       </c>
       <c r="E25" s="29">
-        <v>207670</v>
+        <v>205091</v>
       </c>
       <c r="F25" s="27">
-        <v>137019</v>
+        <v>135567</v>
       </c>
       <c r="G25" s="30">
-        <v>70650</v>
+        <v>69524</v>
       </c>
       <c r="H25" s="31">
-        <v>252048</v>
+        <v>250543</v>
       </c>
       <c r="I25" s="27">
-        <v>203791</v>
+        <v>203406</v>
       </c>
       <c r="J25" s="28">
-        <v>48257</v>
+        <v>47137</v>
       </c>
     </row>
     <row r="26" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57880,31 +57880,31 @@
         <v>15</v>
       </c>
       <c r="B26" s="27">
-        <v>-38008</v>
+        <v>-41639</v>
       </c>
       <c r="C26" s="27">
-        <v>-60404</v>
+        <v>-63702</v>
       </c>
       <c r="D26" s="28">
-        <v>22396</v>
+        <v>22063</v>
       </c>
       <c r="E26" s="29">
-        <v>208061</v>
+        <v>204819</v>
       </c>
       <c r="F26" s="27">
-        <v>138250</v>
+        <v>135701</v>
       </c>
       <c r="G26" s="30">
-        <v>69811</v>
+        <v>69118</v>
       </c>
       <c r="H26" s="31">
-        <v>246069</v>
+        <v>246458</v>
       </c>
       <c r="I26" s="27">
-        <v>198654</v>
+        <v>199403</v>
       </c>
       <c r="J26" s="28">
-        <v>47415</v>
+        <v>47055</v>
       </c>
     </row>
     <row r="27" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57912,31 +57912,31 @@
         <v>16</v>
       </c>
       <c r="B27" s="27">
-        <v>-47243</v>
+        <v>-47157</v>
       </c>
       <c r="C27" s="27">
-        <v>-66506</v>
+        <v>-68718</v>
       </c>
       <c r="D27" s="28">
-        <v>19262</v>
+        <v>21561</v>
       </c>
       <c r="E27" s="29">
-        <v>185114</v>
+        <v>187490</v>
       </c>
       <c r="F27" s="27">
-        <v>127641</v>
+        <v>126875</v>
       </c>
       <c r="G27" s="30">
-        <v>57473</v>
+        <v>60615</v>
       </c>
       <c r="H27" s="31">
-        <v>232357</v>
+        <v>234647</v>
       </c>
       <c r="I27" s="27">
-        <v>194146</v>
+        <v>195594</v>
       </c>
       <c r="J27" s="28">
-        <v>38211</v>
+        <v>39053</v>
       </c>
     </row>
     <row r="28" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57944,31 +57944,31 @@
         <v>17</v>
       </c>
       <c r="B28" s="27">
-        <v>-52611</v>
+        <v>-52959</v>
       </c>
       <c r="C28" s="27">
-        <v>-72302</v>
+        <v>-74616</v>
       </c>
       <c r="D28" s="28">
-        <v>19691</v>
+        <v>21657</v>
       </c>
       <c r="E28" s="29">
-        <v>148770</v>
+        <v>150074</v>
       </c>
       <c r="F28" s="27">
-        <v>95495</v>
+        <v>95025</v>
       </c>
       <c r="G28" s="30">
-        <v>53275</v>
+        <v>55049</v>
       </c>
       <c r="H28" s="31">
-        <v>201381</v>
+        <v>203033</v>
       </c>
       <c r="I28" s="27">
-        <v>167797</v>
+        <v>169641</v>
       </c>
       <c r="J28" s="28">
-        <v>33584</v>
+        <v>33392</v>
       </c>
     </row>
     <row r="29" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57976,31 +57976,31 @@
         <v>18</v>
       </c>
       <c r="B29" s="27">
-        <v>-56310</v>
+        <v>-54915</v>
       </c>
       <c r="C29" s="27">
-        <v>-76733</v>
+        <v>-76652</v>
       </c>
       <c r="D29" s="28">
-        <v>20423</v>
+        <v>21736</v>
       </c>
       <c r="E29" s="29">
-        <v>143679</v>
+        <v>146108</v>
       </c>
       <c r="F29" s="27">
-        <v>89765</v>
+        <v>91051</v>
       </c>
       <c r="G29" s="30">
-        <v>53914</v>
+        <v>55056</v>
       </c>
       <c r="H29" s="31">
-        <v>199990</v>
+        <v>201023</v>
       </c>
       <c r="I29" s="27">
-        <v>166498</v>
+        <v>167703</v>
       </c>
       <c r="J29" s="28">
-        <v>33491</v>
+        <v>33320</v>
       </c>
     </row>
     <row r="30" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -58008,31 +58008,31 @@
         <v>19</v>
       </c>
       <c r="B30" s="27">
-        <v>-51766</v>
+        <v>-50675</v>
       </c>
       <c r="C30" s="27">
-        <v>-72443</v>
+        <v>-72004</v>
       </c>
       <c r="D30" s="28">
-        <v>20677</v>
+        <v>21329</v>
       </c>
       <c r="E30" s="29">
-        <v>157450</v>
+        <v>158805</v>
       </c>
       <c r="F30" s="27">
-        <v>102843</v>
+        <v>103702</v>
       </c>
       <c r="G30" s="30">
-        <v>54606</v>
+        <v>55103</v>
       </c>
       <c r="H30" s="31">
-        <v>209216</v>
+        <v>209480</v>
       </c>
       <c r="I30" s="27">
-        <v>175286</v>
+        <v>175706</v>
       </c>
       <c r="J30" s="28">
-        <v>33930</v>
+        <v>33774</v>
       </c>
     </row>
     <row r="31" spans="1:233" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -58040,31 +58040,31 @@
         <v>20</v>
       </c>
       <c r="B31" s="27">
-        <v>-62110</v>
+        <v>-60743</v>
       </c>
       <c r="C31" s="27">
-        <v>-81517</v>
+        <v>-80792</v>
       </c>
       <c r="D31" s="28">
-        <v>19407</v>
+        <v>20049</v>
       </c>
       <c r="E31" s="29">
-        <v>169876</v>
+        <v>170908</v>
       </c>
       <c r="F31" s="27">
-        <v>115349</v>
+        <v>115880</v>
       </c>
       <c r="G31" s="30">
-        <v>54527</v>
+        <v>55028</v>
       </c>
       <c r="H31" s="31">
-        <v>231986</v>
+        <v>231651</v>
       </c>
       <c r="I31" s="27">
-        <v>196866</v>
+        <v>196672</v>
       </c>
       <c r="J31" s="28">
-        <v>35120</v>
+        <v>34979</v>
       </c>
     </row>
     <row r="32" spans="1:233" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -58072,31 +58072,31 @@
         <v>21</v>
       </c>
       <c r="B32" s="27">
-        <v>-66064</v>
+        <v>-63733</v>
       </c>
       <c r="C32" s="27">
-        <v>-84527</v>
+        <v>-82966</v>
       </c>
       <c r="D32" s="28">
-        <v>18463</v>
+        <v>19233</v>
       </c>
       <c r="E32" s="29">
-        <v>173417</v>
+        <v>174287</v>
       </c>
       <c r="F32" s="27">
-        <v>118787</v>
+        <v>118981</v>
       </c>
       <c r="G32" s="30">
-        <v>54630</v>
+        <v>55306</v>
       </c>
       <c r="H32" s="31">
-        <v>239482</v>
+        <v>238020</v>
       </c>
       <c r="I32" s="27">
-        <v>203314</v>
+        <v>201947</v>
       </c>
       <c r="J32" s="28">
-        <v>36167</v>
+        <v>36073</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -58104,31 +58104,31 @@
         <v>22</v>
       </c>
       <c r="B33" s="27">
-        <v>-63224</v>
+        <v>-62625</v>
       </c>
       <c r="C33" s="27">
-        <v>-81410</v>
+        <v>-81613</v>
       </c>
       <c r="D33" s="28">
-        <v>18187</v>
+        <v>18987</v>
       </c>
       <c r="E33" s="29">
-        <v>177634</v>
+        <v>178063</v>
       </c>
       <c r="F33" s="27">
-        <v>122476</v>
+        <v>121965</v>
       </c>
       <c r="G33" s="30">
-        <v>55158</v>
+        <v>56099</v>
       </c>
       <c r="H33" s="31">
-        <v>240858</v>
+        <v>240689</v>
       </c>
       <c r="I33" s="27">
-        <v>203887</v>
+        <v>203577</v>
       </c>
       <c r="J33" s="28">
-        <v>36971</v>
+        <v>37111</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -58136,31 +58136,31 @@
         <v>23</v>
       </c>
       <c r="B34" s="27">
-        <v>-63978</v>
+        <v>-63678</v>
       </c>
       <c r="C34" s="27">
-        <v>-81944</v>
+        <v>-82127</v>
       </c>
       <c r="D34" s="28">
-        <v>17966</v>
+        <v>18450</v>
       </c>
       <c r="E34" s="29">
-        <v>181616</v>
+        <v>182732</v>
       </c>
       <c r="F34" s="27">
-        <v>126285</v>
+        <v>125761</v>
       </c>
       <c r="G34" s="30">
-        <v>55331</v>
+        <v>56971</v>
       </c>
       <c r="H34" s="31">
-        <v>245594</v>
+        <v>246410</v>
       </c>
       <c r="I34" s="27">
-        <v>208229</v>
+        <v>207888</v>
       </c>
       <c r="J34" s="28">
-        <v>37365</v>
+        <v>38522</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -58168,31 +58168,31 @@
         <v>24</v>
       </c>
       <c r="B35" s="27">
-        <v>-69038</v>
+        <v>-67307</v>
       </c>
       <c r="C35" s="27">
-        <v>-86889</v>
+        <v>-86227</v>
       </c>
       <c r="D35" s="28">
-        <v>17851</v>
+        <v>18920</v>
       </c>
       <c r="E35" s="29">
-        <v>183840</v>
+        <v>185186</v>
       </c>
       <c r="F35" s="27">
-        <v>127638</v>
+        <v>126789</v>
       </c>
       <c r="G35" s="30">
-        <v>56202</v>
+        <v>58397</v>
       </c>
       <c r="H35" s="31">
-        <v>252878</v>
+        <v>252494</v>
       </c>
       <c r="I35" s="27">
-        <v>214528</v>
+        <v>213017</v>
       </c>
       <c r="J35" s="28">
-        <v>38351</v>
+        <v>39477</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -58200,31 +58200,31 @@
         <v>25</v>
       </c>
       <c r="B36" s="27">
-        <v>-66969</v>
+        <v>-65802</v>
       </c>
       <c r="C36" s="27">
-        <v>-84123</v>
+        <v>-84770</v>
       </c>
       <c r="D36" s="28">
-        <v>17155</v>
+        <v>18969</v>
       </c>
       <c r="E36" s="29">
-        <v>190127</v>
+        <v>190877</v>
       </c>
       <c r="F36" s="27">
-        <v>133579</v>
+        <v>131500</v>
       </c>
       <c r="G36" s="30">
-        <v>56548</v>
+        <v>59377</v>
       </c>
       <c r="H36" s="31">
-        <v>257096</v>
+        <v>256678</v>
       </c>
       <c r="I36" s="27">
-        <v>217702</v>
+        <v>216270</v>
       </c>
       <c r="J36" s="28">
-        <v>39394</v>
+        <v>40408</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -58246,31 +58246,31 @@
         <v>13</v>
       </c>
       <c r="B38" s="33">
-        <v>-212789</v>
+        <v>-353070</v>
       </c>
       <c r="C38" s="33">
-        <v>-264710</v>
+        <v>-444504</v>
       </c>
       <c r="D38" s="34">
-        <v>51921</v>
+        <v>91434</v>
       </c>
       <c r="E38" s="35">
-        <v>579851</v>
+        <v>995172</v>
       </c>
       <c r="F38" s="33">
-        <v>410008</v>
+        <v>699196</v>
       </c>
       <c r="G38" s="36">
-        <v>169843</v>
+        <v>295976</v>
       </c>
       <c r="H38" s="37">
-        <v>792640</v>
+        <v>1348242</v>
       </c>
       <c r="I38" s="33">
-        <v>674718</v>
+        <v>1143700</v>
       </c>
       <c r="J38" s="34">
-        <v>117922</v>
+        <v>204542</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -58278,63 +58278,63 @@
         <v>14</v>
       </c>
       <c r="B39" s="27">
-        <v>-67823</v>
+        <v>-67092</v>
       </c>
       <c r="C39" s="27">
-        <v>-85227</v>
+        <v>-86444</v>
       </c>
       <c r="D39" s="28">
-        <v>17404</v>
+        <v>19352</v>
       </c>
       <c r="E39" s="29">
-        <v>192232</v>
+        <v>193221</v>
       </c>
       <c r="F39" s="27">
-        <v>135890</v>
+        <v>134486</v>
       </c>
       <c r="G39" s="30">
-        <v>56342</v>
+        <v>58735</v>
       </c>
       <c r="H39" s="31">
-        <v>260055</v>
+        <v>260313</v>
       </c>
       <c r="I39" s="27">
-        <v>221117</v>
+        <v>220930</v>
       </c>
       <c r="J39" s="28">
-        <v>38938</v>
+        <v>39383</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B40" s="27">
-        <v>-70518</v>
+        <v>-70643</v>
       </c>
       <c r="C40" s="27">
-        <v>-87925</v>
+        <v>-89155</v>
       </c>
       <c r="D40" s="28">
-        <v>17407</v>
+        <v>18513</v>
       </c>
       <c r="E40" s="29">
-        <v>187589</v>
+        <v>188561</v>
       </c>
       <c r="F40" s="27">
-        <v>131231</v>
+        <v>130436</v>
       </c>
       <c r="G40" s="30">
-        <v>56358</v>
+        <v>58125</v>
       </c>
       <c r="H40" s="31">
-        <v>258107</v>
+        <v>259203</v>
       </c>
       <c r="I40" s="27">
-        <v>219156</v>
+        <v>219591</v>
       </c>
       <c r="J40" s="28">
-        <v>38951</v>
+        <v>39612</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -58342,95 +58342,95 @@
         <v>16</v>
       </c>
       <c r="B41" s="27">
-        <v>-74448</v>
+        <v>-75025</v>
       </c>
       <c r="C41" s="27">
-        <v>-91558</v>
+        <v>-92859</v>
       </c>
       <c r="D41" s="28">
-        <v>17109</v>
+        <v>17834</v>
       </c>
       <c r="E41" s="29">
-        <v>200030</v>
+        <v>202669</v>
       </c>
       <c r="F41" s="27">
-        <v>142887</v>
+        <v>143658</v>
       </c>
       <c r="G41" s="30">
-        <v>57143</v>
+        <v>59011</v>
       </c>
       <c r="H41" s="31">
-        <v>274478</v>
+        <v>277693</v>
       </c>
       <c r="I41" s="27">
-        <v>234444</v>
+        <v>236516</v>
       </c>
       <c r="J41" s="28">
-        <v>40034</v>
+        <v>41177</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
-      <c r="B42" s="27" t="s">
-        <v>29</v>
+      <c r="B42" s="27">
+        <v>-69071</v>
       </c>
-      <c r="C42" s="27" t="s">
-        <v>29</v>
+      <c r="C42" s="27">
+        <v>-86873</v>
       </c>
-      <c r="D42" s="28" t="s">
-        <v>29</v>
+      <c r="D42" s="28">
+        <v>17802</v>
       </c>
-      <c r="E42" s="29" t="s">
-        <v>29</v>
+      <c r="E42" s="29">
+        <v>204704</v>
       </c>
-      <c r="F42" s="27" t="s">
-        <v>29</v>
+      <c r="F42" s="27">
+        <v>145088</v>
       </c>
-      <c r="G42" s="30" t="s">
-        <v>29</v>
+      <c r="G42" s="30">
+        <v>59615</v>
       </c>
-      <c r="H42" s="31" t="s">
-        <v>29</v>
+      <c r="H42" s="31">
+        <v>273775</v>
       </c>
-      <c r="I42" s="27" t="s">
-        <v>29</v>
+      <c r="I42" s="27">
+        <v>231961</v>
       </c>
-      <c r="J42" s="28" t="s">
-        <v>29</v>
+      <c r="J42" s="28">
+        <v>41814</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="27" t="s">
-        <v>29</v>
+      <c r="B43" s="27">
+        <v>-71240</v>
       </c>
-      <c r="C43" s="27" t="s">
-        <v>29</v>
+      <c r="C43" s="27">
+        <v>-89174</v>
       </c>
-      <c r="D43" s="28" t="s">
-        <v>29</v>
+      <c r="D43" s="28">
+        <v>17934</v>
       </c>
-      <c r="E43" s="29" t="s">
-        <v>29</v>
+      <c r="E43" s="29">
+        <v>206018</v>
       </c>
-      <c r="F43" s="27" t="s">
-        <v>29</v>
+      <c r="F43" s="27">
+        <v>145528</v>
       </c>
-      <c r="G43" s="30" t="s">
-        <v>29</v>
+      <c r="G43" s="30">
+        <v>60490</v>
       </c>
-      <c r="H43" s="31" t="s">
-        <v>29</v>
+      <c r="H43" s="31">
+        <v>277259</v>
       </c>
-      <c r="I43" s="27" t="s">
-        <v>29</v>
+      <c r="I43" s="27">
+        <v>234702</v>
       </c>
-      <c r="J43" s="28" t="s">
-        <v>29</v>
+      <c r="J43" s="28">
+        <v>42556</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -58674,31 +58674,31 @@
     <row r="52" spans="1:10" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48"/>
       <c r="B52" s="49">
-        <v>-71078</v>
+        <v>-68899</v>
       </c>
       <c r="C52" s="49">
-        <v>-88010</v>
+        <v>-86680</v>
       </c>
       <c r="D52" s="49">
-        <v>16931</v>
+        <v>17781</v>
       </c>
       <c r="E52" s="49">
-        <v>187250</v>
+        <v>204992</v>
       </c>
       <c r="F52" s="49">
-        <v>131131</v>
+        <v>145288</v>
       </c>
       <c r="G52" s="49">
-        <v>56120</v>
+        <v>59704</v>
       </c>
       <c r="H52" s="49">
-        <v>258329</v>
+        <v>273891</v>
       </c>
       <c r="I52" s="49">
-        <v>219140</v>
+        <v>231968</v>
       </c>
       <c r="J52" s="49">
-        <v>39188</v>
+        <v>41923</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="50" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>